<commit_message>
Tuned automatic merging and text replacing
Also, added star parallax effect to null tiles, for no particular reason.
</commit_message>
<xml_diff>
--- a/Documentation/Duchy Upgrades Death Count Table.xlsx
+++ b/Documentation/Duchy Upgrades Death Count Table.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89baa57682530716/Desktop/Mapping/Crusader Kings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\SCRcrusaderkings\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{61EB2A75-3999-42FD-A046-6A5DB3A46D37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BBE88686-3A3B-46CD-BF63-248BD493CA17}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2886AE1-CF88-42C1-B42B-7FCF89A79745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="1485" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14976" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Duchy HP" sheetId="1" r:id="rId1"/>
+    <sheet name="Death Table Duchies" sheetId="3" r:id="rId2"/>
+    <sheet name="Spawns" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="NPA Buttons" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>Duchy HP:</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Stables</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Building:</t>
   </si>
   <si>
@@ -272,6 +269,27 @@
   </si>
   <si>
     <t>Action Kills</t>
+  </si>
+  <si>
+    <t>HP:</t>
+  </si>
+  <si>
+    <t>Original Player</t>
+  </si>
+  <si>
+    <t>Conquering Player</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town </t>
+  </si>
+  <si>
+    <t>0-2</t>
   </si>
 </sst>
 </file>
@@ -309,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +370,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -446,11 +470,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -521,6 +558,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,24 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,18 +925,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99C9B-154D-4D15-A9B9-5300B27EA642}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -881,7 +945,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -890,7 +954,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,19 +962,19 @@
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -930,15 +994,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
@@ -950,128 +1014,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="36">
+        <v>0</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36">
+        <v>0</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="40">
+        <v>0</v>
+      </c>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="43"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30382DBA-5ABD-4D1E-8A8E-4315EC605397}">
-  <dimension ref="A2:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B8:C8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8757BBFC-6C71-4CA4-82E4-CB79EBCBD9A8}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,26 +1117,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>30</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -1128,8 +1160,8 @@
       <c r="F2" s="19">
         <v>1588</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>33</v>
+      <c r="G2" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="19"/>
@@ -1153,8 +1185,8 @@
       <c r="F3" s="27">
         <v>13481</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>34</v>
+      <c r="G3" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -1180,8 +1212,8 @@
       <c r="F4" s="27">
         <v>13474</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>32</v>
+      <c r="G4" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -1209,8 +1241,8 @@
         <f>F4-7</f>
         <v>13467</v>
       </c>
-      <c r="G5" s="32" t="s">
-        <v>31</v>
+      <c r="G5" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1238,8 +1270,8 @@
         <f t="shared" ref="F6:F16" si="1">F5-7</f>
         <v>13460</v>
       </c>
-      <c r="G6" s="33" t="s">
-        <v>73</v>
+      <c r="G6" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -1267,8 +1299,8 @@
         <f t="shared" si="1"/>
         <v>13453</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>35</v>
+      <c r="G7" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20"/>
@@ -1296,8 +1328,8 @@
         <f t="shared" si="1"/>
         <v>13446</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>36</v>
+      <c r="G8" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -1325,8 +1357,8 @@
         <f t="shared" si="1"/>
         <v>13439</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>37</v>
+      <c r="G9" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -1354,8 +1386,8 @@
         <f t="shared" si="1"/>
         <v>13432</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>38</v>
+      <c r="G10" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -1383,8 +1415,8 @@
         <f t="shared" si="1"/>
         <v>13425</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>39</v>
+      <c r="G11" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -1412,8 +1444,8 @@
         <f t="shared" si="1"/>
         <v>13418</v>
       </c>
-      <c r="G12" s="33" t="s">
-        <v>40</v>
+      <c r="G12" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
@@ -1441,8 +1473,8 @@
         <f t="shared" si="1"/>
         <v>13411</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>42</v>
+      <c r="G13" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -1470,8 +1502,8 @@
         <f t="shared" si="1"/>
         <v>13404</v>
       </c>
-      <c r="G14" s="33" t="s">
-        <v>43</v>
+      <c r="G14" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -1499,8 +1531,8 @@
         <f t="shared" si="1"/>
         <v>13397</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>44</v>
+      <c r="G15" s="28" t="s">
+        <v>43</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
@@ -1528,8 +1560,8 @@
         <f t="shared" si="1"/>
         <v>13390</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>41</v>
+      <c r="G16" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
@@ -1543,12 +1575,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94166858-EAEC-47B6-A6C0-FBDAE5212C95}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,24 +1590,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="15">
         <v>2</v>
@@ -1590,7 +1622,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1601,7 +1633,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1612,7 +1644,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1626,7 +1658,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1640,7 +1672,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14">
         <f>SUM(B2:B6)</f>
@@ -1661,7 +1693,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1669,7 +1701,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1680,7 +1712,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1691,7 +1723,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1702,7 +1734,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="14">
         <f>SUM(B8:B11)</f>
@@ -1723,27 +1755,27 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="14">
         <f>SUM(B2+SUM(B13:B16))</f>
@@ -1764,7 +1796,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18">
         <f>SUM(B2+B3+B4+B5+B6+B8+B9+B10+B11+B13+B14+B15+B16)</f>
@@ -1789,6 +1821,103 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30382DBA-5ABD-4D1E-8A8E-4315EC605397}">
+  <dimension ref="A2:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1807,45 +1936,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="B6" s="37"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="31"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Update Duchy Upgrades Death Count Table.xlsx
</commit_message>
<xml_diff>
--- a/Documentation/Duchy Upgrades Death Count Table.xlsx
+++ b/Documentation/Duchy Upgrades Death Count Table.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/89baa57682530716/Desktop/Mapping/Crusader Kings/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\SCRcrusaderkings\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="8_{61EB2A75-3999-42FD-A046-6A5DB3A46D37}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{BBE88686-3A3B-46CD-BF63-248BD493CA17}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2886AE1-CF88-42C1-B42B-7FCF89A79745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4410" yWindow="1485" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14976" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId4"/>
+    <sheet name="Duchy HP" sheetId="1" r:id="rId1"/>
+    <sheet name="Death Table Duchies" sheetId="3" r:id="rId2"/>
+    <sheet name="Spawns" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
     <sheet name="NPA Buttons" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
   <si>
     <t>Duchy HP:</t>
   </si>
@@ -52,9 +52,6 @@
     <t>Stables</t>
   </si>
   <si>
-    <t>N/A</t>
-  </si>
-  <si>
     <t>Building:</t>
   </si>
   <si>
@@ -272,6 +269,27 @@
   </si>
   <si>
     <t>Action Kills</t>
+  </si>
+  <si>
+    <t>HP:</t>
+  </si>
+  <si>
+    <t>Original Player</t>
+  </si>
+  <si>
+    <t>Conquering Player</t>
+  </si>
+  <si>
+    <t>1-9</t>
+  </si>
+  <si>
+    <t>Siege</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Town </t>
+  </si>
+  <si>
+    <t>0-2</t>
   </si>
 </sst>
 </file>
@@ -309,7 +327,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,8 +370,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="8">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -446,11 +470,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -521,6 +558,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -529,24 +610,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -862,18 +925,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99C9B-154D-4D15-A9B9-5300B27EA642}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -881,7 +945,7 @@
         <v>52000</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -890,7 +954,7 @@
         <v>45240</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
@@ -898,19 +962,19 @@
         <v>4</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -930,15 +994,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>9</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>6</v>
@@ -950,128 +1014,96 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>45</v>
-      </c>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="33" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="C13" s="35"/>
+      <c r="D13" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="38" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" s="39"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14" s="36">
+        <v>0</v>
+      </c>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36">
+        <v>0</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="40">
+        <v>0</v>
+      </c>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="34"/>
+      <c r="B15" s="37" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" s="37"/>
+      <c r="D15" s="37" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="37"/>
+      <c r="F15" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="G15" s="43"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30382DBA-5ABD-4D1E-8A8E-4315EC605397}">
-  <dimension ref="A2:F9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7"/>
-      <c r="B2" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" s="8"/>
-    </row>
-    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="28" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
-      <c r="B5" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" s="8"/>
-    </row>
-    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="F3:F4"/>
-    <mergeCell ref="B8:C8"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8757BBFC-6C71-4CA4-82E4-CB79EBCBD9A8}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1085,26 +1117,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="32" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="32" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F1" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" s="31" t="s">
         <v>29</v>
-      </c>
-      <c r="C1" s="36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="36" t="s">
-        <v>78</v>
-      </c>
-      <c r="E1" s="36" t="s">
-        <v>79</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>80</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>30</v>
       </c>
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
@@ -1128,8 +1160,8 @@
       <c r="F2" s="19">
         <v>1588</v>
       </c>
-      <c r="G2" s="33" t="s">
-        <v>33</v>
+      <c r="G2" s="29" t="s">
+        <v>32</v>
       </c>
       <c r="H2" s="20"/>
       <c r="I2" s="19"/>
@@ -1153,8 +1185,8 @@
       <c r="F3" s="27">
         <v>13481</v>
       </c>
-      <c r="G3" s="32" t="s">
-        <v>34</v>
+      <c r="G3" s="28" t="s">
+        <v>33</v>
       </c>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -1180,8 +1212,8 @@
       <c r="F4" s="27">
         <v>13474</v>
       </c>
-      <c r="G4" s="32" t="s">
-        <v>32</v>
+      <c r="G4" s="28" t="s">
+        <v>31</v>
       </c>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -1209,8 +1241,8 @@
         <f>F4-7</f>
         <v>13467</v>
       </c>
-      <c r="G5" s="32" t="s">
-        <v>31</v>
+      <c r="G5" s="28" t="s">
+        <v>30</v>
       </c>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -1238,8 +1270,8 @@
         <f t="shared" ref="F6:F16" si="1">F5-7</f>
         <v>13460</v>
       </c>
-      <c r="G6" s="33" t="s">
-        <v>73</v>
+      <c r="G6" s="29" t="s">
+        <v>72</v>
       </c>
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
@@ -1267,8 +1299,8 @@
         <f t="shared" si="1"/>
         <v>13453</v>
       </c>
-      <c r="G7" s="32" t="s">
-        <v>35</v>
+      <c r="G7" s="28" t="s">
+        <v>34</v>
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="20"/>
@@ -1296,8 +1328,8 @@
         <f t="shared" si="1"/>
         <v>13446</v>
       </c>
-      <c r="G8" s="33" t="s">
-        <v>36</v>
+      <c r="G8" s="29" t="s">
+        <v>35</v>
       </c>
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
@@ -1325,8 +1357,8 @@
         <f t="shared" si="1"/>
         <v>13439</v>
       </c>
-      <c r="G9" s="32" t="s">
-        <v>37</v>
+      <c r="G9" s="28" t="s">
+        <v>36</v>
       </c>
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
@@ -1354,8 +1386,8 @@
         <f t="shared" si="1"/>
         <v>13432</v>
       </c>
-      <c r="G10" s="33" t="s">
-        <v>38</v>
+      <c r="G10" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
@@ -1383,8 +1415,8 @@
         <f t="shared" si="1"/>
         <v>13425</v>
       </c>
-      <c r="G11" s="32" t="s">
-        <v>39</v>
+      <c r="G11" s="28" t="s">
+        <v>38</v>
       </c>
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
@@ -1412,8 +1444,8 @@
         <f t="shared" si="1"/>
         <v>13418</v>
       </c>
-      <c r="G12" s="33" t="s">
-        <v>40</v>
+      <c r="G12" s="29" t="s">
+        <v>39</v>
       </c>
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
@@ -1441,8 +1473,8 @@
         <f t="shared" si="1"/>
         <v>13411</v>
       </c>
-      <c r="G13" s="32" t="s">
-        <v>42</v>
+      <c r="G13" s="28" t="s">
+        <v>41</v>
       </c>
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
@@ -1470,8 +1502,8 @@
         <f t="shared" si="1"/>
         <v>13404</v>
       </c>
-      <c r="G14" s="33" t="s">
-        <v>43</v>
+      <c r="G14" s="29" t="s">
+        <v>42</v>
       </c>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
@@ -1499,8 +1531,8 @@
         <f t="shared" si="1"/>
         <v>13397</v>
       </c>
-      <c r="G15" s="32" t="s">
-        <v>44</v>
+      <c r="G15" s="28" t="s">
+        <v>43</v>
       </c>
       <c r="H15" s="20"/>
       <c r="I15" s="20"/>
@@ -1528,8 +1560,8 @@
         <f t="shared" si="1"/>
         <v>13390</v>
       </c>
-      <c r="G16" s="34" t="s">
-        <v>41</v>
+      <c r="G16" s="30" t="s">
+        <v>40</v>
       </c>
       <c r="H16" s="20"/>
       <c r="I16" s="20"/>
@@ -1543,12 +1575,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94166858-EAEC-47B6-A6C0-FBDAE5212C95}">
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1558,24 +1590,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="D1" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="16" t="s">
         <v>57</v>
-      </c>
-      <c r="E1" s="16" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B2" s="15">
         <v>2</v>
@@ -1590,7 +1622,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1601,7 +1633,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -1612,7 +1644,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1626,7 +1658,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B6">
         <v>3</v>
@@ -1640,7 +1672,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B7" s="14">
         <f>SUM(B2:B6)</f>
@@ -1661,7 +1693,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1669,7 +1701,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9">
         <v>1</v>
@@ -1680,7 +1712,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C10">
         <v>2</v>
@@ -1691,7 +1723,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C11">
         <v>3</v>
@@ -1702,7 +1734,7 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="14">
         <f>SUM(B8:B11)</f>
@@ -1723,27 +1755,27 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B17" s="14">
         <f>SUM(B2+SUM(B13:B16))</f>
@@ -1764,7 +1796,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B18">
         <f>SUM(B2+B3+B4+B5+B6+B8+B9+B10+B11+B13+B14+B15+B16)</f>
@@ -1789,6 +1821,103 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30382DBA-5ABD-4D1E-8A8E-4315EC605397}">
+  <dimension ref="A2:F9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="36" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="44" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="44"/>
+    </row>
+    <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7"/>
+      <c r="B5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="7" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="45"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="B8:C8"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1807,45 +1936,45 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="8"/>
       <c r="B5" s="13" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="37" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="B6" s="37"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="37"/>
+      <c r="B7" s="37"/>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="31"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
-      <c r="B7" s="31"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="31" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="31"/>
+      <c r="B8" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
Diplomacy buildqueue and reset
Set up the diplomacy menu to work with buildqueue detection, and modified the spreadsheet file to calculate the correct buildqueue memory addresses for all players. Attempted to include queue reset action conditions, but they are only partially working and produce visual anomalies.
</commit_message>
<xml_diff>
--- a/Documentation/Duchy Upgrades Death Count Table.xlsx
+++ b/Documentation/Duchy Upgrades Death Count Table.xlsx
@@ -1,25 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Documents\GitHub\SCRcrusaderkings\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\OneDrive\Documents\GitHub\SCRcrusaderkings\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B2886AE1-CF88-42C1-B42B-7FCF89A79745}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A03985D-4BFA-4F85-816D-50D535CD81DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="14976" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
+    <workbookView xWindow="1335" yWindow="2595" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{92E4C457-D108-4D10-A593-E429BDE87694}"/>
   </bookViews>
   <sheets>
     <sheet name="Duchy HP" sheetId="1" r:id="rId1"/>
-    <sheet name="Death Table Duchies" sheetId="3" r:id="rId2"/>
-    <sheet name="Spawns" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
-    <sheet name="NPA Buttons" sheetId="4" r:id="rId5"/>
+    <sheet name="BuildQueueIndexes" sheetId="6" r:id="rId2"/>
+    <sheet name="Death Table Duchies" sheetId="3" r:id="rId3"/>
+    <sheet name="Spawns" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="NPA Buttons" sheetId="4" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="102">
   <si>
     <t>Duchy HP:</t>
   </si>
@@ -290,6 +291,51 @@
   </si>
   <si>
     <t>0-2</t>
+  </si>
+  <si>
+    <t>Base Offset</t>
+  </si>
+  <si>
+    <t>Unit Index</t>
+  </si>
+  <si>
+    <t>Address:</t>
+  </si>
+  <si>
+    <t>!+ Index</t>
+  </si>
+  <si>
+    <t>Node Index</t>
+  </si>
+  <si>
+    <t>Hex Address</t>
+  </si>
+  <si>
+    <t>Player 1</t>
+  </si>
+  <si>
+    <t>Player 2</t>
+  </si>
+  <si>
+    <t>Player 3</t>
+  </si>
+  <si>
+    <t>Player 4</t>
+  </si>
+  <si>
+    <t>Player 5</t>
+  </si>
+  <si>
+    <t>Terran Civilian Build Queue Offsets</t>
+  </si>
+  <si>
+    <t>Build Queue 1/2</t>
+  </si>
+  <si>
+    <t>Build Queue 3/4</t>
+  </si>
+  <si>
+    <t>Build Queue 5 (?)</t>
   </si>
 </sst>
 </file>
@@ -327,7 +373,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -376,8 +422,44 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -483,11 +565,33 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -527,16 +631,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -561,7 +661,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -575,6 +675,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -584,24 +702,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -610,6 +710,63 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -927,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDC99C9B-154D-4D15-A9B9-5300B27EA642}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -1033,65 +1190,65 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="33" t="s">
+      <c r="A13" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="35" t="s">
+      <c r="B13" s="39" t="s">
         <v>86</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35" t="s">
+      <c r="C13" s="39"/>
+      <c r="D13" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="E13" s="35"/>
-      <c r="F13" s="38" t="s">
+      <c r="E13" s="39"/>
+      <c r="F13" s="33" t="s">
         <v>83</v>
       </c>
-      <c r="G13" s="39"/>
+      <c r="G13" s="34"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="34" t="s">
+      <c r="A14" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="36">
+      <c r="B14" s="40">
         <v>0</v>
       </c>
-      <c r="C14" s="36"/>
-      <c r="D14" s="36">
+      <c r="C14" s="40"/>
+      <c r="D14" s="40">
         <v>0</v>
       </c>
-      <c r="E14" s="36"/>
-      <c r="F14" s="40">
+      <c r="E14" s="40"/>
+      <c r="F14" s="35">
         <v>0</v>
       </c>
-      <c r="G14" s="41"/>
+      <c r="G14" s="36"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="34"/>
-      <c r="B15" s="37" t="s">
+      <c r="A15" s="32"/>
+      <c r="B15" s="41" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="37" t="s">
+      <c r="C15" s="41"/>
+      <c r="D15" s="41" t="s">
         <v>82</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="42" t="s">
+      <c r="E15" s="41"/>
+      <c r="F15" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="G15" s="43"/>
+      <c r="G15" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="F15:G15"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="F14:G14"/>
-    <mergeCell ref="F15:G15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1099,6 +1256,266 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4D0E2967-5063-4C0C-B615-7C0652627782}">
+  <dimension ref="A1:K7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="2" width="14.7109375" customWidth="1"/>
+    <col min="3" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B1" s="51"/>
+      <c r="C1" s="51"/>
+      <c r="D1" s="51"/>
+      <c r="E1" s="51"/>
+      <c r="F1" s="52" t="s">
+        <v>99</v>
+      </c>
+      <c r="G1" s="52"/>
+      <c r="H1" s="53" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="53"/>
+      <c r="J1" s="64" t="s">
+        <v>101</v>
+      </c>
+      <c r="K1" s="65"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="50" t="s">
+        <v>87</v>
+      </c>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="50" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" s="50" t="s">
+        <v>90</v>
+      </c>
+      <c r="F2" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="50" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>5885248</v>
+      </c>
+      <c r="B3" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="46">
+        <v>156</v>
+      </c>
+      <c r="D3" s="46">
+        <f>1699-(C3-1)</f>
+        <v>1544</v>
+      </c>
+      <c r="E3" s="46">
+        <f>336*D3</f>
+        <v>518784</v>
+      </c>
+      <c r="F3" s="55">
+        <f>$A$3+E3</f>
+        <v>6404032</v>
+      </c>
+      <c r="G3" s="56" t="str">
+        <f>DEC2HEX(F3)</f>
+        <v>61B7C0</v>
+      </c>
+      <c r="H3" s="57">
+        <f>F3+4</f>
+        <v>6404036</v>
+      </c>
+      <c r="I3" s="58" t="str">
+        <f>DEC2HEX(H3)</f>
+        <v>61B7C4</v>
+      </c>
+      <c r="J3" s="54"/>
+      <c r="K3" s="54"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="63" t="str">
+        <f>DEC2HEX(A3)</f>
+        <v>59CD40</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4" s="48">
+        <v>157</v>
+      </c>
+      <c r="D4" s="46">
+        <f t="shared" ref="D4:D7" si="0">1699-(C4-1)</f>
+        <v>1543</v>
+      </c>
+      <c r="E4" s="48">
+        <f t="shared" ref="E4:E7" si="1">336*D4</f>
+        <v>518448</v>
+      </c>
+      <c r="F4" s="59">
+        <f>$A$3+E4</f>
+        <v>6403696</v>
+      </c>
+      <c r="G4" s="60" t="str">
+        <f t="shared" ref="G4:G7" si="2">DEC2HEX(F4)</f>
+        <v>61B670</v>
+      </c>
+      <c r="H4" s="61">
+        <f t="shared" ref="H4:H7" si="3">F4+4</f>
+        <v>6403700</v>
+      </c>
+      <c r="I4" s="62" t="str">
+        <f t="shared" ref="I4:I7" si="4">DEC2HEX(H4)</f>
+        <v>61B674</v>
+      </c>
+      <c r="J4" s="54"/>
+      <c r="K4" s="54"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="45">
+        <v>158</v>
+      </c>
+      <c r="D5" s="46">
+        <f t="shared" si="0"/>
+        <v>1542</v>
+      </c>
+      <c r="E5" s="49">
+        <f t="shared" si="1"/>
+        <v>518112</v>
+      </c>
+      <c r="F5" s="45">
+        <f>$A$3+E5</f>
+        <v>6403360</v>
+      </c>
+      <c r="G5" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>61B520</v>
+      </c>
+      <c r="H5" s="54">
+        <f t="shared" si="3"/>
+        <v>6403364</v>
+      </c>
+      <c r="I5" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>61B524</v>
+      </c>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="45">
+        <v>159</v>
+      </c>
+      <c r="D6" s="46">
+        <f t="shared" si="0"/>
+        <v>1541</v>
+      </c>
+      <c r="E6" s="49">
+        <f t="shared" si="1"/>
+        <v>517776</v>
+      </c>
+      <c r="F6" s="45">
+        <f>$A$3+E6</f>
+        <v>6403024</v>
+      </c>
+      <c r="G6" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>61B3D0</v>
+      </c>
+      <c r="H6" s="54">
+        <f t="shared" si="3"/>
+        <v>6403028</v>
+      </c>
+      <c r="I6" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>61B3D4</v>
+      </c>
+      <c r="J6" s="54"/>
+      <c r="K6" s="54"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="45">
+        <v>160</v>
+      </c>
+      <c r="D7" s="46">
+        <f t="shared" si="0"/>
+        <v>1540</v>
+      </c>
+      <c r="E7" s="49">
+        <f t="shared" si="1"/>
+        <v>517440</v>
+      </c>
+      <c r="F7" s="45">
+        <f>$A$3+E7</f>
+        <v>6402688</v>
+      </c>
+      <c r="G7" s="47" t="str">
+        <f t="shared" si="2"/>
+        <v>61B280</v>
+      </c>
+      <c r="H7" s="54">
+        <f t="shared" si="3"/>
+        <v>6402692</v>
+      </c>
+      <c r="I7" s="47" t="str">
+        <f t="shared" si="4"/>
+        <v>61B284</v>
+      </c>
+      <c r="J7" s="54"/>
+      <c r="K7" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8757BBFC-6C71-4CA4-82E4-CB79EBCBD9A8}">
   <dimension ref="A1:I16"/>
   <sheetViews>
@@ -1117,29 +1534,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="32" t="s">
+      <c r="D1" s="30" t="s">
         <v>77</v>
       </c>
-      <c r="E1" s="32" t="s">
+      <c r="E1" s="30" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="30" t="s">
         <v>79</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="17">
@@ -1148,104 +1563,97 @@
       <c r="B2" s="18">
         <v>1</v>
       </c>
-      <c r="C2" s="19">
+      <c r="C2" s="12">
         <v>19027</v>
       </c>
-      <c r="D2" s="19">
+      <c r="D2" s="12">
         <v>1585</v>
       </c>
       <c r="E2">
         <v>19060</v>
       </c>
-      <c r="F2" s="19">
+      <c r="F2" s="12">
         <v>1588</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="G2" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="20"/>
-      <c r="I2" s="19"/>
+      <c r="I2" s="12"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="25">
+      <c r="A3" s="23">
         <v>1</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="24">
         <v>2</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="25">
         <v>161743</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="25">
         <v>13478</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="22">
         <v>161776</v>
       </c>
-      <c r="F3" s="27">
+      <c r="F3" s="25">
         <v>13481</v>
       </c>
-      <c r="G3" s="28" t="s">
+      <c r="G3" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="25">
+      <c r="A4" s="23">
         <v>2</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="24">
         <v>3</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="25">
         <f>C3-84</f>
         <v>161659</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="25">
         <f>D3-7</f>
         <v>13471</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="25">
         <v>161692</v>
       </c>
-      <c r="F4" s="27">
+      <c r="F4" s="25">
         <v>13474</v>
       </c>
-      <c r="G4" s="28" t="s">
+      <c r="G4" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="H4" s="20"/>
-      <c r="I4" s="20"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="25">
+      <c r="A5" s="23">
         <v>3</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="24">
         <v>4</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="25">
         <f>C4-84</f>
         <v>161575</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="25">
         <f>D4-7</f>
         <v>13464</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="25">
         <f>E4-84</f>
         <v>161608</v>
       </c>
-      <c r="F5" s="27">
+      <c r="F5" s="25">
         <f>F4-7</f>
         <v>13467</v>
       </c>
-      <c r="G5" s="28" t="s">
+      <c r="G5" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="17">
@@ -1254,56 +1662,53 @@
       <c r="B6" s="18">
         <v>5</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="12">
         <f>C5-84</f>
         <v>161491</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="12">
         <f>D5-7</f>
         <v>13457</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="25">
         <f t="shared" ref="E6:E16" si="0">E5-84</f>
         <v>161524</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="12">
         <f t="shared" ref="F6:F16" si="1">F5-7</f>
         <v>13460</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="25">
+      <c r="A7" s="23">
         <v>5</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>6</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="25">
         <f>C6-84</f>
         <v>161407</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="25">
         <f>D6-7</f>
         <v>13450</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="25">
         <f t="shared" si="0"/>
         <v>161440</v>
       </c>
-      <c r="F7" s="27">
+      <c r="F7" s="25">
         <f t="shared" si="1"/>
         <v>13453</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="19"/>
-      <c r="I7" s="20"/>
+      <c r="H7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="17">
@@ -1312,56 +1717,52 @@
       <c r="B8" s="18">
         <v>7</v>
       </c>
-      <c r="C8" s="19">
+      <c r="C8" s="12">
         <f>C7-84</f>
         <v>161323</v>
       </c>
-      <c r="D8" s="19">
+      <c r="D8" s="12">
         <f t="shared" ref="D8:D16" si="2">D7-7</f>
         <v>13443</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="25">
         <f t="shared" si="0"/>
         <v>161356</v>
       </c>
-      <c r="F8" s="19">
+      <c r="F8" s="12">
         <f t="shared" si="1"/>
         <v>13446</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="25">
+      <c r="A9" s="23">
         <v>7</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>8</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="25">
         <f t="shared" ref="C9:C16" si="3">C8-84</f>
         <v>161239</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="25">
         <f t="shared" si="2"/>
         <v>13436</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="25">
         <f t="shared" si="0"/>
         <v>161272</v>
       </c>
-      <c r="F9" s="27">
+      <c r="F9" s="25">
         <f t="shared" si="1"/>
         <v>13439</v>
       </c>
-      <c r="G9" s="28" t="s">
+      <c r="G9" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="H9" s="20"/>
-      <c r="I9" s="20"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="17">
@@ -1370,56 +1771,52 @@
       <c r="B10" s="18">
         <v>9</v>
       </c>
-      <c r="C10" s="19">
+      <c r="C10" s="12">
         <f t="shared" si="3"/>
         <v>161155</v>
       </c>
-      <c r="D10" s="19">
+      <c r="D10" s="12">
         <f t="shared" si="2"/>
         <v>13429</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="25">
         <f t="shared" si="0"/>
         <v>161188</v>
       </c>
-      <c r="F10" s="19">
+      <c r="F10" s="12">
         <f t="shared" si="1"/>
         <v>13432</v>
       </c>
-      <c r="G10" s="29" t="s">
+      <c r="G10" s="27" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="25">
+      <c r="A11" s="23">
         <v>9</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="24">
         <v>10</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="25">
         <f t="shared" si="3"/>
         <v>161071</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="25">
         <f t="shared" si="2"/>
         <v>13422</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="25">
         <f t="shared" si="0"/>
         <v>161104</v>
       </c>
-      <c r="F11" s="27">
+      <c r="F11" s="25">
         <f t="shared" si="1"/>
         <v>13425</v>
       </c>
-      <c r="G11" s="28" t="s">
+      <c r="G11" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="20"/>
-      <c r="I11" s="20"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
@@ -1428,56 +1825,52 @@
       <c r="B12" s="18">
         <v>11</v>
       </c>
-      <c r="C12" s="19">
+      <c r="C12" s="12">
         <f t="shared" si="3"/>
         <v>160987</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="12">
         <f t="shared" si="2"/>
         <v>13415</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="25">
         <f t="shared" si="0"/>
         <v>161020</v>
       </c>
-      <c r="F12" s="19">
+      <c r="F12" s="12">
         <f t="shared" si="1"/>
         <v>13418</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H12" s="20"/>
-      <c r="I12" s="20"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="25">
+      <c r="A13" s="23">
         <v>11</v>
       </c>
-      <c r="B13" s="26">
+      <c r="B13" s="24">
         <v>12</v>
       </c>
-      <c r="C13" s="27">
+      <c r="C13" s="25">
         <f t="shared" si="3"/>
         <v>160903</v>
       </c>
-      <c r="D13" s="27">
+      <c r="D13" s="25">
         <f t="shared" si="2"/>
         <v>13408</v>
       </c>
-      <c r="E13" s="27">
+      <c r="E13" s="25">
         <f t="shared" si="0"/>
         <v>160936</v>
       </c>
-      <c r="F13" s="27">
+      <c r="F13" s="25">
         <f t="shared" si="1"/>
         <v>13411</v>
       </c>
-      <c r="G13" s="28" t="s">
+      <c r="G13" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="17">
@@ -1486,85 +1879,79 @@
       <c r="B14" s="18">
         <v>13</v>
       </c>
-      <c r="C14" s="19">
+      <c r="C14" s="12">
         <f t="shared" si="3"/>
         <v>160819</v>
       </c>
-      <c r="D14" s="19">
+      <c r="D14" s="12">
         <f t="shared" si="2"/>
         <v>13401</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="25">
         <f t="shared" si="0"/>
         <v>160852</v>
       </c>
-      <c r="F14" s="19">
+      <c r="F14" s="12">
         <f t="shared" si="1"/>
         <v>13404</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
+      <c r="A15" s="23">
         <v>13</v>
       </c>
-      <c r="B15" s="26">
+      <c r="B15" s="24">
         <v>14</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="25">
         <f t="shared" si="3"/>
         <v>160735</v>
       </c>
-      <c r="D15" s="27">
+      <c r="D15" s="25">
         <f t="shared" si="2"/>
         <v>13394</v>
       </c>
-      <c r="E15" s="27">
+      <c r="E15" s="25">
         <f t="shared" si="0"/>
         <v>160768</v>
       </c>
-      <c r="F15" s="27">
+      <c r="F15" s="25">
         <f t="shared" si="1"/>
         <v>13397</v>
       </c>
-      <c r="G15" s="28" t="s">
+      <c r="G15" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="21">
+      <c r="A16" s="19">
         <v>14</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="20">
         <v>15</v>
       </c>
-      <c r="C16" s="23">
+      <c r="C16" s="21">
         <f t="shared" si="3"/>
         <v>160651</v>
       </c>
-      <c r="D16" s="23">
+      <c r="D16" s="21">
         <f t="shared" si="2"/>
         <v>13387</v>
       </c>
-      <c r="E16" s="27">
+      <c r="E16" s="25">
         <f t="shared" si="0"/>
         <v>160684</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="21">
         <f t="shared" si="1"/>
         <v>13390</v>
       </c>
-      <c r="G16" s="30" t="s">
+      <c r="G16" s="28" t="s">
         <v>40</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1575,7 +1962,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94166858-EAEC-47B6-A6C0-FBDAE5212C95}">
   <dimension ref="A1:F18"/>
   <sheetViews>
@@ -1824,7 +2211,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30382DBA-5ABD-4D1E-8A8E-4315EC605397}">
   <dimension ref="A2:F9"/>
   <sheetViews>
@@ -1858,7 +2245,7 @@
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
-      <c r="F3" s="44" t="s">
+      <c r="F3" s="42" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1870,7 +2257,7 @@
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
-      <c r="F4" s="44"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7"/>
@@ -1897,8 +2284,8 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="36" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="45"/>
-      <c r="C8" s="46"/>
+      <c r="B8" s="43"/>
+      <c r="C8" s="44"/>
       <c r="D8" s="11" t="s">
         <v>16</v>
       </c>
@@ -1921,12 +2308,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79E0B7D0-8170-4324-AFB2-A8BBC4DA1105}">
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,20 +2348,20 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="41" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="37"/>
+      <c r="B6" s="41"/>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="37"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="41"/>
+      <c r="B7" s="41"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="41" t="s">
         <v>51</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>